<commit_message>
v6 - QA, matched demo
</commit_message>
<xml_diff>
--- a/statements.xlsx
+++ b/statements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrymanley/Desktop/Classes/PAM4540/cMapKMeans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117E1955-1A04-7045-AC87-270F67644334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541B6F0F-532E-594C-8685-C27B4C6ACD10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11340" yWindow="740" windowWidth="18940" windowHeight="16080" xr2:uid="{81DE784C-55A9-8F45-BEC6-DADBD43F1E67}"/>
+    <workbookView xWindow="7120" yWindow="480" windowWidth="18940" windowHeight="16080" activeTab="1" xr2:uid="{81DE784C-55A9-8F45-BEC6-DADBD43F1E67}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30718710-F170-8A46-9DEB-73AC2148897F}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACE2343-1E29-5645-8393-97AD81596C90}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>